<commit_message>
Update the about table.
</commit_message>
<xml_diff>
--- a/data/Fertility Rate By Ethnic Group, Yearly.xlsx
+++ b/data/Fertility Rate By Ethnic Group, Yearly.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jeremy\PortableR\RPortableWorkDirectory\QuartoDash\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jeremy\PortableR\RPortableWorkDirectory\fertility_dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC24426-6F87-4C2E-A4CC-AC56B4903622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79ABCED9-B4EF-4ADC-8FD6-50B204AED1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1812" windowWidth="20004" windowHeight="10704" xr2:uid="{E5D317DC-364D-46FD-82B1-C49EE70CDD7C}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{E5D317DC-364D-46FD-82B1-C49EE70CDD7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -250,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.##########"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,17 +259,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -280,7 +272,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -288,40 +280,24 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -639,9 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F879DCA7-02B3-42E7-8D41-E74E4423FB5A}">
   <dimension ref="A1:BM5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -649,204 +623,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BA1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BB1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BC1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BD1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BE1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BF1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BG1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BH1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BI1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BK1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BL1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BM1" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="4">
@@ -1002,13 +976,13 @@
       <c r="AZ2" s="4">
         <v>2.79</v>
       </c>
-      <c r="BA2" s="2">
+      <c r="BA2" s="5">
         <v>3</v>
       </c>
       <c r="BB2" s="4">
         <v>2.98</v>
       </c>
-      <c r="BC2" s="2">
+      <c r="BC2" s="5">
         <v>3</v>
       </c>
       <c r="BD2" s="4">
@@ -1043,7 +1017,7 @@
       </c>
     </row>
     <row r="3" spans="1:65" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>67</v>
       </c>
       <c r="B3" s="4">
@@ -1240,7 +1214,7 @@
       </c>
     </row>
     <row r="4" spans="1:65" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B4" s="4">
@@ -1258,10 +1232,10 @@
       <c r="F4" s="4">
         <v>0.98</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="5">
         <v>1</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="5">
         <v>1</v>
       </c>
       <c r="I4" s="4">

</xml_diff>